<commit_message>
push code import excel mentor, student, admin dashboard
</commit_message>
<xml_diff>
--- a/importMentor.xlsx
+++ b/importMentor.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trinhquocthang/Documents/Workspace/Project/Topic-13-FE/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3B18D0-C331-AD4F-A42F-AAD963B4729F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="28800" yWindow="-9240" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -64,9 +73,6 @@
     <t>ME102023</t>
   </si>
   <si>
-    <t>Python,Spring Boot</t>
-  </si>
-  <si>
     <t>mentor2</t>
   </si>
   <si>
@@ -85,9 +91,6 @@
     <t>ME102002</t>
   </si>
   <si>
-    <t>.NET,Python</t>
-  </si>
-  <si>
     <t>mentor3</t>
   </si>
   <si>
@@ -106,37 +109,53 @@
     <t>ME102003</t>
   </si>
   <si>
-    <t>Python</t>
+    <t>React, NodeJs</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>Deploy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -144,51 +163,55 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -378,26 +401,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="21.25"/>
-    <col customWidth="1" min="3" max="3" width="14.13"/>
-    <col customWidth="1" min="9" max="9" width="17.5"/>
-    <col customWidth="1" min="10" max="10" width="23.38"/>
+    <col min="2" max="2" width="21.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="9" max="9" width="17.5" customWidth="1"/>
+    <col min="10" max="10" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -429,7 +457,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -443,13 +471,13 @@
         <v>13</v>
       </c>
       <c r="E2" s="3">
-        <v>33018.0</v>
+        <v>33018</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="2">
-        <v>9.1239192E7</v>
+        <v>91239192</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>15</v>
@@ -457,75 +485,75 @@
       <c r="I2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="E3" s="3">
-        <v>33018.0</v>
+        <v>33018</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="2">
-        <v>2.345678901E9</v>
+        <v>2345678901</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" s="3">
+        <v>32369</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="3">
-        <v>32369.0</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="G4" s="2">
-        <v>3.456789012E9</v>
+        <v>3456789012</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -537,7 +565,7 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -549,7 +577,7 @@
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -561,7 +589,7 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -573,7 +601,7 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -585,13 +613,13 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E10" s="3"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E11" s="3"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
push change pass for admin and fix return list null
</commit_message>
<xml_diff>
--- a/importMentor.xlsx
+++ b/importMentor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trinhquocthang/Documents/Workspace/Project/Topic-13-FE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3B18D0-C331-AD4F-A42F-AAD963B4729F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6790D3-BF4F-6845-93F7-E7D2651C75AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-9240" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Username</t>
   </si>
@@ -28,9 +28,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Password</t>
-  </si>
-  <si>
     <t>Full Name</t>
   </si>
   <si>
@@ -58,9 +55,6 @@
     <t>mentor1@gmail.com</t>
   </si>
   <si>
-    <t>password1</t>
-  </si>
-  <si>
     <t>Alex Smith</t>
   </si>
   <si>
@@ -79,9 +73,6 @@
     <t>mentor2@gmail.com</t>
   </si>
   <si>
-    <t>password2</t>
-  </si>
-  <si>
     <t>Jane Smith</t>
   </si>
   <si>
@@ -95,9 +86,6 @@
   </si>
   <si>
     <t>mentor3@gmail.com</t>
-  </si>
-  <si>
-    <t>password3</t>
   </si>
   <si>
     <t>Alex Johnson</t>
@@ -411,21 +399,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="21.1640625" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" customWidth="1"/>
-    <col min="9" max="9" width="17.5" customWidth="1"/>
-    <col min="10" max="10" width="23.33203125" customWidth="1"/>
+    <col min="8" max="8" width="17.5" customWidth="1"/>
+    <col min="9" max="9" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,171 +440,154 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="3">
+        <v>33018</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2">
+        <v>91239192</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="3">
+      <c r="H2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="3">
         <v>33018</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="2">
-        <v>91239192</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2345678901</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="I3" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="3">
-        <v>33018</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="2">
-        <v>2345678901</v>
-      </c>
-      <c r="H3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
+      <c r="D4" s="3">
+        <v>32369</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="F4" s="2">
+        <v>3456789012</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="3">
-        <v>32369</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="I4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="2">
-        <v>3456789012</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="6"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="6"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="6"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="6"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="6"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E11" s="3"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>